<commit_message>
Pre To Post Code Updated
</commit_message>
<xml_diff>
--- a/DataFiles/CMS/Excel/post_pre_migration.xlsx
+++ b/DataFiles/CMS/Excel/post_pre_migration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RaptrDXP\Selenium\CRM_REQUESTS\DataFiles\CMS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDF79B4-4BBA-442C-8A6E-9F5467044225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C28C3C-7C93-4EBB-8C58-60D6C46DE50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A45345F0-DCA7-4A49-8398-E60D370244B7}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="169">
   <si>
     <t>search_by</t>
   </si>
@@ -587,6 +587,12 @@
   </si>
   <si>
     <t>Customer request is created successfully.</t>
+  </si>
+  <si>
+    <t>prepaid_plan_name</t>
+  </si>
+  <si>
+    <t>9Talk</t>
   </si>
 </sst>
 </file>
@@ -654,7 +660,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -686,13 +692,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1"/>
@@ -700,6 +717,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
@@ -1151,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF75EBE2-1F39-4454-A6E6-3A1251D4A838}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,9 +1182,10 @@
     <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1182,8 +1201,11 @@
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F1" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1195,6 +1217,9 @@
       </c>
       <c r="E2" t="s">
         <v>166</v>
+      </c>
+      <c r="F2" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>